<commit_message>
Added remove option, plot, splited in classes
</commit_message>
<xml_diff>
--- a/OPCUaClass/ConnectionApp/tabel.xlsx
+++ b/OPCUaClass/ConnectionApp/tabel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="B1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,170 +434,56 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Machinetype</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Protocol</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Endpoint</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>AddressNs</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>mdescription</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>IP</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Arburg</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>OPC UA</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>host_computer</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>opc.tcp://10.210.40.215:4880/Arburg</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>dataSS.csv</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Arburg</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>OPC UA</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>opc.tcp://10.210.40.219:4880/Arburg</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>dataSS.csv</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Fanuc</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>EU 63</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>M614</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>x.x.x.x.x</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Arburg</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>OPC UA</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>host_computer</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>opc.tcp://10.210.40.215:4880/Arburg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>dataSS.csv</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed the delete option, added plot, EU63 implmementation in progress
</commit_message>
<xml_diff>
--- a/OPCUaClass/ConnectionApp/tabel.xlsx
+++ b/OPCUaClass/ConnectionApp/tabel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:K1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,54 +434,107 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.3</t>
+          <t>Machinetype</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.2</t>
+          <t>Protocol</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.1</t>
+          <t>Username</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Password</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Machinetype</t>
+          <t>Endpoint</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Protocol</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Endpoint</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
           <t>AddressNs</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Arburg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OPC UA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>host_computer</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>opc.tcp://10.210.40.219:4880/Arburg</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>dataSS.csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Arburg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OPC UA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>host_computer</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>opc.tcp://10.210.40.215:4880/Arburg</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>dataSS.csv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed a loop bug, changed a bit the interface
</commit_message>
<xml_diff>
--- a/OPCUaClass/ConnectionApp/tabel.xlsx
+++ b/OPCUaClass/ConnectionApp/tabel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>AddressNs</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>mdescription</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -504,6 +514,8 @@
           <t>dataSS.csv</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -535,6 +547,35 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>dataSS.csv</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fanuc</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EU 63</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>M614</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>x.x.x.x.x</t>
         </is>
       </c>
     </row>

</xml_diff>